<commit_message>
Added User, Lecture, and Course classes. Also got Shopping Cart frame to list out a course in the table
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
   <si>
     <t>kvw5270</t>
   </si>
@@ -24,6 +24,90 @@
   </si>
   <si>
     <t>02/09/2020 23:28:44</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Invalid Username!</t>
+  </si>
+  <si>
+    <t>02/22/2020 15:39:22</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:00:59</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:25:44</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:26:31</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:27:39</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:28:03</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:29:17</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:29:34</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:31:16</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:35:44</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:37:38</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:39:06</t>
+  </si>
+  <si>
+    <t>02/22/2020 22:39:26</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:09:20</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:10:14</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:16:50</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:18:20</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:20:37</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:23:19</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:23:59</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:24:19</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:43:56</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:46:37</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:47:22</t>
+  </si>
+  <si>
+    <t>02/23/2020 00:49:07</t>
   </si>
 </sst>
 </file>
@@ -68,18 +152,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.37109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0234375" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed repository Netbeans added into pom.xml.Added additionalCourseInfoWindow to pop up when double clicking a row. Fixed windows so that they open up in the center of the screen. Working on improving additionalCourseInfoWindow functionality as well as saving User data and loading it in (using serializable interface).
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="55">
   <si>
     <t>kvw5270</t>
   </si>
@@ -108,6 +108,75 @@
   </si>
   <si>
     <t>02/23/2020 00:49:07</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:22:40</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:24:00</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:24:25</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:25:12</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:25:42</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:26:02</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:26:21</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:27:57</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:31:36</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:32:16</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:57:43</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:58:57</t>
+  </si>
+  <si>
+    <t>02/23/2020 11:59:22</t>
+  </si>
+  <si>
+    <t>02/23/2020 12:06:34</t>
+  </si>
+  <si>
+    <t>02/23/2020 12:07:30</t>
+  </si>
+  <si>
+    <t>02/23/2020 12:10:30</t>
+  </si>
+  <si>
+    <t>02/23/2020 12:12:33</t>
+  </si>
+  <si>
+    <t>02/23/2020 13:59:22</t>
+  </si>
+  <si>
+    <t>02/23/2020 13:59:44</t>
+  </si>
+  <si>
+    <t>02/23/2020 14:02:27</t>
+  </si>
+  <si>
+    <t>02/23/2020 14:09:58</t>
+  </si>
+  <si>
+    <t>02/23/2020 14:10:32</t>
+  </si>
+  <si>
+    <t>02/23/2020 14:12:02</t>
   </si>
 </sst>
 </file>
@@ -175,7 +244,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Currently getting NoClassDefFoundError when trying to run jar. Meanwhile, updated additionalCourseInfoWindow so that it is able to generate a hardcoded table. Will eventually update so that it prints all sections of a course as well as an add button to add to ShoppingCart for User.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="71">
   <si>
     <t>kvw5270</t>
   </si>
@@ -177,6 +177,54 @@
   </si>
   <si>
     <t>02/23/2020 14:12:02</t>
+  </si>
+  <si>
+    <t>02/23/2020 14:15:30</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:20:33</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:20:44</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:22:56</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:23:30</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:24:05</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:24:21</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:24:59</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:27:39</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:29:10</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:30:11</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:30:25</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:31:24</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:31:52</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:32:35</t>
+  </si>
+  <si>
+    <t>02/23/2020 15:32:53</t>
   </si>
 </sst>
 </file>
@@ -244,7 +292,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SchedulingSystem class. Additionally renamed additionalCourseInfoWindow to CourseInfoWindow. Will spend time this upcoming break cleaning up the packages and re evaluating how they all interact.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="96">
   <si>
     <t>kvw5270</t>
   </si>
@@ -225,6 +225,81 @@
   </si>
   <si>
     <t>02/23/2020 15:32:53</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:19:01</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:22:26</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:25:03</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:27:12</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:31:05</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:37:25</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:37:45</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:38:53</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:39:06</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:39:34</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:40:28</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:40:48</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:41:09</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:43:13</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:56:02</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:56:24</t>
+  </si>
+  <si>
+    <t>03/02/2020 01:57:51</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:01:23</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:13:21</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:36:50</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:37:22</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:38:06</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:38:35</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:40:06</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:40:33</t>
   </si>
 </sst>
 </file>
@@ -292,7 +367,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Main class. Renamed User to Student for better readability. Updated SchedulingSystem with more attributes and methods for usability. Also added an AdministratorWindow for adding and removing Courses.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="118">
   <si>
     <t>kvw5270</t>
   </si>
@@ -300,6 +300,72 @@
   </si>
   <si>
     <t>03/02/2020 02:40:33</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:51:47</t>
+  </si>
+  <si>
+    <t>03/02/2020 02:52:30</t>
+  </si>
+  <si>
+    <t>03/02/2020 03:03:31</t>
+  </si>
+  <si>
+    <t>03/09/2020 23:30:16</t>
+  </si>
+  <si>
+    <t>03/13/2020 19:24:14</t>
+  </si>
+  <si>
+    <t>03/13/2020 19:29:31</t>
+  </si>
+  <si>
+    <t>03/13/2020 19:45:06</t>
+  </si>
+  <si>
+    <t>03/13/2020 19:59:01</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:13:27</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:19:21</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:19:32</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:22:50</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:23:01</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:30:09</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:32:53</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:35:25</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:36:37</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:36:50</t>
+  </si>
+  <si>
+    <t>03/13/2020 20:53:10</t>
+  </si>
+  <si>
+    <t>03/14/2020 14:22:56</t>
+  </si>
+  <si>
+    <t>03/14/2020 14:23:08</t>
+  </si>
+  <si>
+    <t>03/14/2020 14:29:10</t>
   </si>
 </sst>
 </file>
@@ -367,7 +433,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added AddCourseWindow and AddSectionsWindow that allow administrator to add Courses and Sections to those Courses into the Scheduling System.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="122">
   <si>
     <t>kvw5270</t>
   </si>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t>03/14/2020 14:29:10</t>
+  </si>
+  <si>
+    <t>03/14/2020 16:43:19</t>
+  </si>
+  <si>
+    <t>03/14/2020 21:48:06</t>
+  </si>
+  <si>
+    <t>03/14/2020 21:48:25</t>
+  </si>
+  <si>
+    <t>03/14/2020 21:48:58</t>
   </si>
 </sst>
 </file>
@@ -433,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added working search functionality for the ShoppingCart. Also started working on updating the CourseInfoWindow so that it meets specifications.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="135">
   <si>
     <t>kvw5270</t>
   </si>
@@ -378,6 +378,45 @@
   </si>
   <si>
     <t>03/14/2020 21:48:58</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>03/16/2020 09:52:53</t>
+  </si>
+  <si>
+    <t>03/16/2020 10:31:50</t>
+  </si>
+  <si>
+    <t>03/16/2020 10:32:32</t>
+  </si>
+  <si>
+    <t>03/22/2020 21:26:27</t>
+  </si>
+  <si>
+    <t>03/22/2020 22:18:53</t>
+  </si>
+  <si>
+    <t>03/22/2020 22:20:35</t>
+  </si>
+  <si>
+    <t>03/22/2020 22:21:03</t>
+  </si>
+  <si>
+    <t>03/22/2020 22:22:12</t>
+  </si>
+  <si>
+    <t>03/22/2020 22:22:49</t>
+  </si>
+  <si>
+    <t>03/22/2020 22:23:27</t>
+  </si>
+  <si>
+    <t>03/22/2020 23:08:58</t>
+  </si>
+  <si>
+    <t>03/22/2020 23:09:36</t>
   </si>
 </sst>
 </file>
@@ -428,7 +467,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.37109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.234375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="20.0234375" collapsed="true"/>
   </cols>
   <sheetData>
@@ -442,10 +481,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Currently a lot of windows not working. Working on getting the Scheduling System passed between windows so that it may be updated and saved properly.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="144">
   <si>
     <t>kvw5270</t>
   </si>
@@ -417,6 +417,33 @@
   </si>
   <si>
     <t>03/22/2020 23:09:36</t>
+  </si>
+  <si>
+    <t>03/22/2020 23:14:29</t>
+  </si>
+  <si>
+    <t>03/22/2020 23:14:43</t>
+  </si>
+  <si>
+    <t>03/23/2020 21:44:21</t>
+  </si>
+  <si>
+    <t>03/23/2020 21:45:22</t>
+  </si>
+  <si>
+    <t>03/23/2020 22:15:12</t>
+  </si>
+  <si>
+    <t>03/23/2020 22:18:01</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>03/23/2020 22:34:51</t>
+  </si>
+  <si>
+    <t>03/23/2020 22:38:38</t>
   </si>
 </sst>
 </file>
@@ -481,10 +508,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Able show course information in CourseInfoWindow now
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="147">
   <si>
     <t>kvw5270</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>03/23/2020 22:38:38</t>
+  </si>
+  <si>
+    <t>03/24/2020 00:53:58</t>
+  </si>
+  <si>
+    <t>03/24/2020 00:59:25</t>
+  </si>
+  <si>
+    <t>03/24/2020 01:00:57</t>
   </si>
 </sst>
 </file>
@@ -508,10 +517,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CourseInfoWindow prints exactly as requested by client, updated with checkmarks.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="152">
   <si>
     <t>kvw5270</t>
   </si>
@@ -453,6 +453,21 @@
   </si>
   <si>
     <t>03/24/2020 01:00:57</t>
+  </si>
+  <si>
+    <t>03/24/2020 01:09:08</t>
+  </si>
+  <si>
+    <t>03/24/2020 01:10:03</t>
+  </si>
+  <si>
+    <t>03/24/2020 01:10:16</t>
+  </si>
+  <si>
+    <t>03/24/2020 01:10:29</t>
+  </si>
+  <si>
+    <t>03/24/2020 01:12:32</t>
   </si>
 </sst>
 </file>
@@ -503,16 +518,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.234375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="20.0234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2">
@@ -520,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made column width for selection checkmarks in AddCourseWindow a more acceptable size. AddCourseWindow is also no longer resizable to the user.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="179">
   <si>
     <t>kvw5270</t>
   </si>
@@ -468,6 +468,87 @@
   </si>
   <si>
     <t>03/24/2020 01:12:32</t>
+  </si>
+  <si>
+    <t>03/24/2020 10:01:00</t>
+  </si>
+  <si>
+    <t>03/24/2020 10:03:00</t>
+  </si>
+  <si>
+    <t>03/24/2020 10:04:41</t>
+  </si>
+  <si>
+    <t>03/24/2020 10:05:03</t>
+  </si>
+  <si>
+    <t>03/24/2020 10:05:50</t>
+  </si>
+  <si>
+    <t>03/24/2020 10:07:19</t>
+  </si>
+  <si>
+    <t>03/24/2020 10:09:19</t>
+  </si>
+  <si>
+    <t>03/30/2020 22:36:53</t>
+  </si>
+  <si>
+    <t>03/30/2020 22:52:07</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:01:57</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:02:16</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:03:39</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:05:37</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:07:03</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:08:48</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:09:44</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:10:04</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:11:16</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:11:44</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:13:57</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:14:32</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:15:17</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:15:48</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:18:23</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:19:47</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:22:16</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:23:53</t>
   </si>
 </sst>
 </file>
@@ -535,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separated DateTime so that Date and Time are separate strings allowing for more flexibility.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="191">
   <si>
     <t>kvw5270</t>
   </si>
@@ -549,6 +549,42 @@
   </si>
   <si>
     <t>03/30/2020 23:23:53</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:46:25</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:48:30</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:49:53</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:51:02</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:51:41</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:52:46</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:53:05</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:53:46</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:54:04</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:54:34</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:56:39</t>
+  </si>
+  <si>
+    <t>03/30/2020 23:57:28</t>
   </si>
 </sst>
 </file>
@@ -616,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally able to generate executable Jar file. Turns out I don't need to use the Fully Qualified Name when defining the Main class in the pom.xml file? Two Jar files are created so use the one that is created with dependencies.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>Username</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>04/06/2020 00:01:33</t>
+  </si>
+  <si>
+    <t>04/08/2020 08:40:06</t>
+  </si>
+  <si>
+    <t>04/08/2020 10:02:04</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved issue with printing Courses info in ShoppingCartWindow: was calling getSection from Course object instead of getEnrolledSection from Student object. Also added starting jFrames for a QueuePositionWindow and a window that alerts the user to when a QueueJump occurs.
</commit_message>
<xml_diff>
--- a/SchedulerProgram/students.xlsx
+++ b/SchedulerProgram/students.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -45,6 +45,48 @@
   </si>
   <si>
     <t>04/14/2020 00:33:41</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:41:05</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:41:29</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:41:43</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:42:55</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:43:25</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:46:39</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:48:52</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:49:21</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:49:27</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:49:32</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:51:29</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:51:46</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:51:53</t>
+  </si>
+  <si>
+    <t>04/14/2020 00:51:59</t>
   </si>
 </sst>
 </file>
@@ -113,13 +155,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>